<commit_message>
New Feature - Deleted annotation
Breaking Change
- TestSpec.xlsx is replaced
</commit_message>
<xml_diff>
--- a/src/main/resources/TestSpec.xlsx
+++ b/src/main/resources/TestSpec.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03972674-FB70-0C41-A54E-384204242961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259549DE-A631-6647-8012-A6B52A2D31E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="3900" windowWidth="39920" windowHeight="28500" activeTab="2" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
+    <workbookView xWindow="31960" yWindow="5300" windowWidth="39920" windowHeight="28500" activeTab="3" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
   <sheets>
     <sheet name="CommandList" sheetId="1" r:id="rId1"/>
     <sheet name="Summary" sheetId="2" r:id="rId2"/>
-    <sheet name="TestSpec" sheetId="3" r:id="rId3"/>
-    <sheet name="List" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Template" sheetId="5" r:id="rId3"/>
+    <sheet name="TestSpec" sheetId="3" r:id="rId4"/>
+    <sheet name="List" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="実施結果">List!$A$3:$A$12</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -388,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,6 +507,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,7 +805,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1061,6 +1068,57 @@
     <xf numFmtId="49" fontId="11" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="21" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1069,7 +1127,7 @@
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1" xr:uid="{C40AA10B-FA57-1748-8D8E-3E12991DC054}"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="41">
     <dxf>
       <fill>
         <patternFill>
@@ -1115,14 +1173,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFA0D8EF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1136,7 +1194,120 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA0D8EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEE82EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBDD7EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1157,182 +1328,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFEE82EE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1353,30 +1349,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1389,9 +1361,35 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1406,101 +1404,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBDD7EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCCFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA0D8EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA0D8EF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEE82EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -1509,68 +1412,6 @@
       <font>
         <b/>
         <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
   </dxfs>
@@ -1971,8 +1812,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="22">
-      <c r="A1" s="102"/>
-      <c r="B1" s="102"/>
+      <c r="A1" s="119"/>
+      <c r="B1" s="119"/>
       <c r="C1" s="13" t="s">
         <v>40</v>
       </c>
@@ -6474,78 +6315,13 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="74" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="D4:O104">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 F4:G104 K4:O104">
-    <cfRule type="cellIs" dxfId="73" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="72" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="70" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="69" priority="10" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G104">
-    <cfRule type="cellIs" dxfId="68" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D104">
-    <cfRule type="cellIs" dxfId="67" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6:E104">
-    <cfRule type="cellIs" dxfId="66" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J4:J104">
-    <cfRule type="cellIs" dxfId="65" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="64" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H104">
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:H104">
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I104">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="G4:H104">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6554,14 +6330,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641B8779-49CC-7C41-8244-DBC27C6FCB57}">
-  <dimension ref="A1:S1009"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5517B1B6-F75C-9849-81BE-13D42D1EB82F}">
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="4" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" sqref="A1:C1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.28515625" defaultRowHeight="14" outlineLevelRow="1"/>
@@ -6587,9 +6363,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1" ht="22">
-      <c r="A1" s="102"/>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="A1" s="119"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
       <c r="D1" s="13"/>
       <c r="E1" s="14"/>
       <c r="F1" s="93"/>
@@ -6801,7 +6577,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="43">
-        <f t="shared" ref="A10:A73" si="0">ROW()-9</f>
+        <f t="shared" ref="A10:A19" si="0">ROW()-9</f>
         <v>1</v>
       </c>
       <c r="B10" s="44"/>
@@ -6850,6 +6626,567 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="B12" s="111"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="113"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="118"/>
+      <c r="P12" s="112"/>
+      <c r="Q12" s="112"/>
+      <c r="R12" s="112"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="43">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="102"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="108"/>
+      <c r="L13" s="107"/>
+      <c r="M13" s="108"/>
+      <c r="N13" s="107"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="110"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="43">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="43">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="43">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="43">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="55"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="43">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <conditionalFormatting sqref="E1">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="51">
+      <formula>LEN(TRIM(E1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="containsText" dxfId="37" priority="11" operator="containsText" text="iOS">
+      <formula>NOT(ISERROR(SEARCH("iOS",G11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="Android">
+      <formula>NOT(ISERROR(SEARCH("Android",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13:G19">
+    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Android">
+      <formula>NOT(ISERROR(SEARCH("Android",G13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="24" operator="containsText" text="iOS">
+      <formula>NOT(ISERROR(SEARCH("iOS",G13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
+    <cfRule type="cellIs" dxfId="33" priority="49" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="32" priority="13" operator="equal">
+      <formula>"手動"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I19">
+    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
+      <formula>"手動"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J19">
+    <cfRule type="containsText" dxfId="30" priority="9" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="10" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+      <formula>NOT(ISERROR(SEARCH("NOTIMPL",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="8" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",J10)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"未実施"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J10:J19" xr:uid="{1560CB35-642B-4243-BC7E-84F2E510B678}">
+      <formula1>実施結果</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13:G19 G11" xr:uid="{DD8963A1-EF3E-1941-81DF-E83E95667E82}">
+      <formula1>"iOS,Android"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641B8779-49CC-7C41-8244-DBC27C6FCB57}">
+  <dimension ref="A1:S1009"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="4" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.28515625" defaultRowHeight="14" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="20" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="57" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="9" style="24" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="25" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="25" customWidth="1"/>
+    <col min="13" max="14" width="8.140625" style="25" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" style="25" customWidth="1"/>
+    <col min="16" max="17" width="8.140625" style="25" customWidth="1"/>
+    <col min="18" max="18" width="29.28515625" style="26" customWidth="1"/>
+    <col min="19" max="20" width="8" style="20" customWidth="1"/>
+    <col min="21" max="16384" width="6.28515625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="22">
+      <c r="A1" s="119"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="17"/>
+    </row>
+    <row r="2" spans="1:19" ht="17" customHeight="1" outlineLevel="1">
+      <c r="C2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="20"/>
+    </row>
+    <row r="3" spans="1:19" ht="14" customHeight="1" outlineLevel="1">
+      <c r="C3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" spans="1:19" ht="14" customHeight="1" outlineLevel="1">
+      <c r="C4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="31"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="20"/>
+    </row>
+    <row r="5" spans="1:19" ht="14" customHeight="1" outlineLevel="1">
+      <c r="C5" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="31"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="20"/>
+    </row>
+    <row r="6" spans="1:19" ht="14" customHeight="1" outlineLevel="1">
+      <c r="C6" s="32"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="20"/>
+    </row>
+    <row r="7" spans="1:19" ht="14" customHeight="1">
+      <c r="C7" s="32"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="J7" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="38">
+        <f>SUM(H4,H5,H6,K3,K4,K5,K6)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="20"/>
+    </row>
+    <row r="8" spans="1:19" ht="14" customHeight="1">
+      <c r="C8" s="32"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="20"/>
+    </row>
+    <row r="9" spans="1:19" ht="36.75" customHeight="1">
+      <c r="A9" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="43">
+        <f t="shared" ref="A10:A73" si="0">ROW()-9</f>
+        <v>1</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="99"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="96"/>
+      <c r="Q10" s="96"/>
+      <c r="R10" s="96"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="43">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="43">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="B12" s="47"/>
       <c r="C12" s="48"/>
       <c r="D12" s="49"/>
@@ -29804,124 +30141,59 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="I11 I13 I15 I17 I19 I21 I23 I25 I27 I29 I31 I33 I35 I37 I39 I41 I43 I45 I47 I49 I51 I53 I55 I99 I143 I187 I231 I275 I319 I363 I407 I451 I495 I57 I101 I145 I189 I233 I277 I321 I365 I409 I453 I497 I59 I103 I147 I191 I235 I279 I323 I367 I411 I455 I499 I61 I105 I149 I193 I237 I281 I325 I369 I413 I457 I501 I63 I107 I151 I195 I239 I283 I327 I371 I415 I459 I65 I109 I153 I197 I241 I285 I329 I373 I417 I461 I67 I111 I155 I199 I243 I287 I331 I375 I419 I463 I69 I113 I157 I201 I245 I289 I333 I377 I421 I465 I71 I115 I159 I203 I247 I291 I335 I379 I423 I467 I73 I117 I161 I205 I249 I293 I337 I381 I425 I469 I75 I119 I163 I207 I251 I295 I339 I383 I427 I471 I77 I121 I165 I209 I253 I297 I341 I385 I429 I473 I79 I123 I167 I211 I255 I299 I343 I387 I431 I475 I81 I125 I169 I213 I257 I301 I345 I389 I433 I477 I83 I127 I171 I215 I259 I303 I347 I391 I435 I479 I85 I129 I173 I217 I261 I305 I349 I393 I437 I481 I87 I131 I175 I219 I263 I307 I351 I395 I439 I483 I89 I133 I177 I221 I265 I309 I353 I397 I441 I485 I91 I135 I179 I223 I267 I311 I355 I399 I443 I487 I93 I137 I181 I225 I269 I313 I357 I401 I445 I489 I95 I139 I183 I227 I271 I315 I359 I403 I447 I491 I97 I141 I185 I229 I273 I317 I361 I405 I449 I493 I503 I505 I507 I509">
-    <cfRule type="cellIs" dxfId="59" priority="40" operator="equal">
+  <conditionalFormatting sqref="E1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="51">
+      <formula>LEN(TRIM(E1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G1009">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="Android">
+      <formula>NOT(ISERROR(SEARCH("Android",G11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="iOS">
+      <formula>NOT(ISERROR(SEARCH("iOS",G11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
+    <cfRule type="cellIs" dxfId="17" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I1009">
+    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
       <formula>"手動"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12 I14 I16 I18 I20 I22 I24 I26 I28 I30 I32 I34 I36 I38 I40 I42 I44 I46 I48 I50 I52 I54 I56 I100 I144 I188 I232 I276 I320 I364 I408 I452 I496 I58 I102 I146 I190 I234 I278 I322 I366 I410 I454 I498 I60 I104 I148 I192 I236 I280 I324 I368 I412 I456 I500 I62 I106 I150 I194 I238 I282 I326 I370 I414 I458 I502 I64 I108 I152 I196 I240 I284 I328 I372 I416 I460 I66 I110 I154 I198 I242 I286 I330 I374 I418 I462 I68 I112 I156 I200 I244 I288 I332 I376 I420 I464 I70 I114 I158 I202 I246 I290 I334 I378 I422 I466 I72 I116 I160 I204 I248 I292 I336 I380 I424 I468 I74 I118 I162 I206 I250 I294 I338 I382 I426 I470 I76 I120 I164 I208 I252 I296 I340 I384 I428 I472 I78 I122 I166 I210 I254 I298 I342 I386 I430 I474 I80 I124 I168 I212 I256 I300 I344 I388 I432 I476 I82 I126 I170 I214 I258 I302 I346 I390 I434 I478 I84 I128 I172 I216 I260 I304 I348 I392 I436 I480 I86 I130 I174 I218 I262 I306 I350 I394 I438 I482 I88 I132 I176 I220 I264 I308 I352 I396 I440 I484 I90 I134 I178 I222 I266 I310 I354 I398 I442 I486 I92 I136 I180 I224 I268 I312 I356 I400 I444 I488 I94 I138 I182 I226 I270 I314 I358 I402 I446 I490 I96 I140 I184 I228 I272 I316 I360 I404 I448 I492 I98 I142 I186 I230 I274 I318 I362 I406 I450 I494 I504 I506 I508">
-    <cfRule type="cellIs" dxfId="58" priority="39" operator="equal">
-      <formula>"手動"</formula>
+  <conditionalFormatting sqref="J10:J1009">
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"実施対象外"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J11">
-    <cfRule type="cellIs" dxfId="57" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"削除予定"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="8" stopIfTrue="1" operator="containsText" text="ERROR">
+      <formula>NOT(ISERROR(SEARCH("ERROR",J10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="9" stopIfTrue="1" operator="containsText" text="SKIP">
+      <formula>NOT(ISERROR(SEARCH("SKIP",J10)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>"未実施"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="36" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",J10)))</formula>
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"保留"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="37" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",J10)))</formula>
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"MANUAL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="38" stopIfTrue="1" operator="containsText" text="NOTIMPL">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"NG"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" stopIfTrue="1" operator="containsText" text="NOTIMPL">
       <formula>NOT(ISERROR(SEARCH("NOTIMPL",J10)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J11">
-    <cfRule type="cellIs" dxfId="53" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="31" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="33" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="34" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="35" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J11">
-    <cfRule type="cellIs" dxfId="48" priority="32" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="28">
-      <formula>LEN(TRIM(E1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I511 I513 I515 I517 I519 I521 I523 I525 I527 I529 I531 I533 I535 I537 I539 I541 I543 I545 I547 I549 I551 I553 I555 I599 I643 I687 I731 I775 I819 I863 I907 I951 I995 I557 I601 I645 I689 I733 I777 I821 I865 I909 I953 I997 I559 I603 I647 I691 I735 I779 I823 I867 I911 I955 I999 I561 I605 I649 I693 I737 I781 I825 I869 I913 I957 I1001 I563 I607 I651 I695 I739 I783 I827 I871 I915 I959 I565 I609 I653 I697 I741 I785 I829 I873 I917 I961 I567 I611 I655 I699 I743 I787 I831 I875 I919 I963 I569 I613 I657 I701 I745 I789 I833 I877 I921 I965 I571 I615 I659 I703 I747 I791 I835 I879 I923 I967 I573 I617 I661 I705 I749 I793 I837 I881 I925 I969 I575 I619 I663 I707 I751 I795 I839 I883 I927 I971 I577 I621 I665 I709 I753 I797 I841 I885 I929 I973 I579 I623 I667 I711 I755 I799 I843 I887 I931 I975 I581 I625 I669 I713 I757 I801 I845 I889 I933 I977 I583 I627 I671 I715 I759 I803 I847 I891 I935 I979 I585 I629 I673 I717 I761 I805 I849 I893 I937 I981 I587 I631 I675 I719 I763 I807 I851 I895 I939 I983 I589 I633 I677 I721 I765 I809 I853 I897 I941 I985 I591 I635 I679 I723 I767 I811 I855 I899 I943 I987 I593 I637 I681 I725 I769 I813 I857 I901 I945 I989 I595 I639 I683 I727 I771 I815 I859 I903 I947 I991 I597 I641 I685 I729 I773 I817 I861 I905 I949 I993 I1003 I1005 I1007 I1009">
-    <cfRule type="cellIs" dxfId="46" priority="27" operator="equal">
-      <formula>"手動"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I512 I514 I516 I518 I520 I522 I524 I526 I528 I530 I532 I534 I536 I538 I540 I542 I544 I546 I548 I550 I552 I554 I556 I600 I644 I688 I732 I776 I820 I864 I908 I952 I996 I558 I602 I646 I690 I734 I778 I822 I866 I910 I954 I998 I560 I604 I648 I692 I736 I780 I824 I868 I912 I956 I1000 I562 I606 I650 I694 I738 I782 I826 I870 I914 I958 I1002 I564 I608 I652 I696 I740 I784 I828 I872 I916 I960 I566 I610 I654 I698 I742 I786 I830 I874 I918 I962 I568 I612 I656 I700 I744 I788 I832 I876 I920 I964 I570 I614 I658 I702 I746 I790 I834 I878 I922 I966 I572 I616 I660 I704 I748 I792 I836 I880 I924 I968 I574 I618 I662 I706 I750 I794 I838 I882 I926 I970 I576 I620 I664 I708 I752 I796 I840 I884 I928 I972 I578 I622 I666 I710 I754 I798 I842 I886 I930 I974 I580 I624 I668 I712 I756 I800 I844 I888 I932 I976 I582 I626 I670 I714 I758 I802 I846 I890 I934 I978 I584 I628 I672 I716 I760 I804 I848 I892 I936 I980 I586 I630 I674 I718 I762 I806 I850 I894 I938 I982 I588 I632 I676 I720 I764 I808 I852 I896 I940 I984 I590 I634 I678 I722 I766 I810 I854 I898 I942 I986 I592 I636 I680 I724 I768 I812 I856 I900 I944 I988 I594 I638 I682 I726 I770 I814 I858 I902 I946 I990 I596 I640 I684 I728 I772 I816 I860 I904 I948 I992 I598 I642 I686 I730 I774 I818 I862 I906 I950 I994 I1004 I1006 I1008">
-    <cfRule type="cellIs" dxfId="45" priority="26" operator="equal">
-      <formula>"手動"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I510">
-    <cfRule type="cellIs" dxfId="44" priority="25" operator="equal">
-      <formula>"手動"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="43" priority="24" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:J1009">
-    <cfRule type="cellIs" dxfId="41" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="10" stopIfTrue="1" operator="containsText" text="ERROR">
-      <formula>NOT(ISERROR(SEARCH("ERROR",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="11" stopIfTrue="1" operator="containsText" text="SKIP">
-      <formula>NOT(ISERROR(SEARCH("SKIP",J12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="12" stopIfTrue="1" operator="containsText" text="NOTIMPL">
-      <formula>NOT(ISERROR(SEARCH("NOTIMPL",J12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:J1009">
-    <cfRule type="cellIs" dxfId="37" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J12:J1009">
-    <cfRule type="cellIs" dxfId="32" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"MANUAL"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G1009">
-    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="iOS">
-      <formula>NOT(ISERROR(SEARCH("iOS",G11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="Android">
-      <formula>NOT(ISERROR(SEARCH("Android",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -29936,7 +30208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC8D3DF-4B4C-6241-B3EE-09F2029151AE}">
   <dimension ref="A2:B22"/>
   <sheetViews>
@@ -30037,87 +30309,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="A3:A8">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
-      <formula>"削除予定"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
-      <formula>"実施対象外"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"保留"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"NG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
-      <formula>"未実施"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
+  <conditionalFormatting sqref="A3:A12">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"削除予定"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Improvement - SpecReport - SummaryReport
</commit_message>
<xml_diff>
--- a/src/main/resources/TestSpec.xlsx
+++ b/src/main/resources/TestSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wave1008/github/ldi-github/shirates-core/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2523753-5397-5148-8282-02034E22D39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4275A2BF-BF01-624F-9AC8-DE969C079750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="39920" windowHeight="36460" activeTab="1" xr2:uid="{7D8110C6-6013-EE40-AEFD-DB3E77751E94}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>result</t>
     <phoneticPr fontId="5"/>
@@ -279,6 +279,14 @@
   <si>
     <t>A+CA+M</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>NLR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mode</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1748,7 +1756,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18F45A1-E8E7-6045-B22A-269DB8A60478}">
-  <dimension ref="A3:L3"/>
+  <dimension ref="A3:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1759,20 +1767,21 @@
   <cols>
     <col min="1" max="1" width="5.5703125" style="95" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="95" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="95" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="95" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="95" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="95" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="95" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" style="95" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="95" customWidth="1"/>
-    <col min="10" max="10" width="51.7109375" style="95" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="95" customWidth="1"/>
-    <col min="12" max="12" width="43" style="95" customWidth="1"/>
-    <col min="13" max="16384" width="10.7109375" style="95"/>
+    <col min="3" max="4" width="10.140625" style="95" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="95" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" style="95" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="95" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="95" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" style="95" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="95" customWidth="1"/>
+    <col min="11" max="11" width="51.7109375" style="95" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="95" customWidth="1"/>
+    <col min="13" max="13" width="43" style="95" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" style="95" customWidth="1"/>
+    <col min="15" max="16384" width="10.7109375" style="95"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="95" t="s">
         <v>47</v>
       </c>
@@ -1783,31 +1792,37 @@
         <v>49</v>
       </c>
       <c r="D3" s="95" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="F3" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="G3" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="95" t="s">
+      <c r="H3" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="95" t="s">
+      <c r="I3" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="95" t="s">
+      <c r="J3" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="95" t="s">
+      <c r="K3" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="95" t="s">
+      <c r="L3" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="95" t="s">
+      <c r="M3" s="95" t="s">
         <v>56</v>
+      </c>
+      <c r="N3" s="95" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -9326,6 +9341,10 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="I2" s="20"/>
+      <c r="J2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="28"/>
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
@@ -9341,10 +9360,10 @@
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
       <c r="I3" s="20"/>
-      <c r="J3" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="28"/>
+      <c r="J3" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="31"/>
       <c r="L3" s="20"/>
       <c r="M3" s="20"/>
       <c r="N3" s="20"/>
@@ -9887,6 +9906,10 @@
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
       <c r="I2" s="20"/>
+      <c r="J2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="28"/>
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
@@ -9902,10 +9925,10 @@
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
       <c r="I3" s="20"/>
-      <c r="J3" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="28"/>
+      <c r="J3" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="31"/>
       <c r="L3" s="20"/>
       <c r="M3" s="20"/>
       <c r="N3" s="20"/>

</xml_diff>